<commit_message>
fix: minor detial fixes, compact db
</commit_message>
<xml_diff>
--- a/accessdb/Registry/defaultFamSheet.xlsx
+++ b/accessdb/Registry/defaultFamSheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\zebwin11pc\networkdb\Registry\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Jovial\Workspace\GitHub\joe733\cbcefdb\accessdb\networkdb\Registry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{503DBB47-13F9-497F-BB9E-748EE32B241F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D59784-D5A3-4D6D-9CD8-61E5714036DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="26385" windowHeight="14235" xr2:uid="{691864EF-CD39-4A4F-A743-1915A8367D6B}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="FamilyRegister" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">FamilyRegister!$A$1:$I$60</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">FamilyRegister!$A$1:$I$61</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">FamilyRegister!$A:$G,FamilyRegister!$5:$5</definedName>
   </definedNames>
   <calcPr calcId="181029" iterate="1"/>
@@ -460,7 +460,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t xml:space="preserve">ക്രിസ്ത്യന്‍ ബ്രദറണ്‍ ചര്‍ച്ച് ഈസ്റ്റ് ഫോര്‍ട്ട്‌ </t>
   </si>
@@ -650,6 +650,12 @@
   <si>
     <t>Member 7</t>
   </si>
+  <si>
+    <t>പാസ്പോർട്ട് ഫോട്ടോ</t>
+  </si>
+  <si>
+    <t>ഫാമിലി ഫോട്ടോ:</t>
+  </si>
 </sst>
 </file>
 
@@ -786,7 +792,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -877,6 +883,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -987,74 +999,10 @@
         <vertAlign val="baseline"/>
         <sz val="11"/>
         <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="0"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1106,10 +1054,74 @@
         <vertAlign val="baseline"/>
         <sz val="11"/>
         <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
         <scheme val="none"/>
       </font>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1125,11 +1137,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{7ED75F74-C5D4-4B51-8775-6C43A3A144B1}" name="Table4" displayName="Table4" ref="A5:I47" headerRowDxfId="10" dataDxfId="8" totalsRowDxfId="9">
-  <autoFilter ref="A5:I47" xr:uid="{7ED75F74-C5D4-4B51-8775-6C43A3A144B1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{7ED75F74-C5D4-4B51-8775-6C43A3A144B1}" name="Table4" displayName="Table4" ref="A5:I48" headerRowDxfId="13" dataDxfId="12" totalsRowDxfId="11">
+  <autoFilter ref="A5:I48" xr:uid="{7ED75F74-C5D4-4B51-8775-6C43A3A144B1}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{6D668163-801A-41BB-B009-B9F1EBB13689}" name="Sl. No." totalsRowLabel="Total" dataDxfId="11" totalsRowDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{BF741685-7980-46D2-B60C-07F0984CB8EA}" name="Description" dataDxfId="7" totalsRowDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{6D668163-801A-41BB-B009-B9F1EBB13689}" name="Sl. No." totalsRowLabel="Total" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{BF741685-7980-46D2-B60C-07F0984CB8EA}" name="Description" dataDxfId="8" totalsRowDxfId="7"/>
     <tableColumn id="3" xr3:uid="{F4DDDD5A-3EBA-47E6-A236-E0C7A8103AA5}" name="Member 1" dataDxfId="6"/>
     <tableColumn id="4" xr3:uid="{8F749AF5-81B8-4352-AA35-80B088E8E5B4}" name="Member 2" dataDxfId="5"/>
     <tableColumn id="5" xr3:uid="{75367B76-F1C6-4FD6-82A3-2C15368DDF06}" name="Member 3" dataDxfId="4"/>
@@ -1439,10 +1451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B0EA35-602C-4E1F-A94E-665F1CEBDA8B}">
-  <dimension ref="A1:I1015"/>
+  <dimension ref="A1:I1016"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1476,6 +1488,9 @@
       <c r="E2" s="30"/>
       <c r="F2" s="30"/>
       <c r="G2" s="30"/>
+      <c r="H2" s="15" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="3" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="5"/>
@@ -2115,29 +2130,33 @@
     </row>
     <row r="47" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="16">
-        <v>21</v>
+        <v>29</v>
       </c>
-      <c r="B47" s="17" t="s">
+      <c r="B47" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C47" s="32"/>
+      <c r="D47" s="32"/>
+      <c r="E47" s="32"/>
+      <c r="F47" s="32"/>
+      <c r="G47" s="32"/>
+      <c r="H47" s="32"/>
+      <c r="I47" s="32"/>
+    </row>
+    <row r="48" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="16">
+        <v>30</v>
+      </c>
+      <c r="B48" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="27"/>
-      <c r="G47" s="27"/>
-      <c r="H47" s="27"/>
-      <c r="I47" s="27"/>
-    </row>
-    <row r="48" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="2"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="6"/>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6"/>
-      <c r="I48" s="6"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="27"/>
+      <c r="E48" s="27"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
+      <c r="H48" s="27"/>
+      <c r="I48" s="27"/>
     </row>
     <row r="49" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2"/>
@@ -2152,23 +2171,23 @@
     </row>
     <row r="50" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2"/>
-      <c r="B50" s="23" t="s">
-        <v>45</v>
-      </c>
+      <c r="B50" s="1"/>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
-      <c r="G50" s="7"/>
-      <c r="H50" s="7"/>
-      <c r="I50" s="7"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="6"/>
     </row>
     <row r="51" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="19"/>
+      <c r="B51" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C51" s="6"/>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
       <c r="G51" s="7"/>
       <c r="H51" s="7"/>
       <c r="I51" s="7"/>
@@ -2176,24 +2195,24 @@
     <row r="52" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
       <c r="B52" s="1"/>
-      <c r="C52" s="6"/>
+      <c r="C52" s="19"/>
       <c r="D52" s="6"/>
-      <c r="E52" s="7"/>
-      <c r="H52" s="20" t="s">
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="7"/>
+      <c r="I52" s="7"/>
+    </row>
+    <row r="53" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="2"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="7"/>
+      <c r="H53" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="I52" s="8"/>
-    </row>
-    <row r="53" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="2"/>
-      <c r="B53" s="9"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="10"/>
-      <c r="E53" s="7"/>
-      <c r="H53" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="I53" s="11"/>
+      <c r="I53" s="8"/>
     </row>
     <row r="54" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
@@ -2202,36 +2221,36 @@
       <c r="D54" s="10"/>
       <c r="E54" s="7"/>
       <c r="H54" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I54" s="11"/>
     </row>
     <row r="55" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="12"/>
+      <c r="A55" s="2"/>
       <c r="B55" s="9"/>
       <c r="C55" s="10"/>
       <c r="D55" s="10"/>
       <c r="E55" s="7"/>
       <c r="H55" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="I55" s="11"/>
+    </row>
+    <row r="56" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="12"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="7"/>
+      <c r="H56" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="I55" s="11"/>
-    </row>
-    <row r="56" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="12"/>
-      <c r="B56" s="24" t="s">
+      <c r="I56" s="11"/>
+    </row>
+    <row r="57" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="12"/>
+      <c r="B57" s="24" t="s">
         <v>50</v>
-      </c>
-      <c r="C56" s="7"/>
-      <c r="D56" s="7"/>
-      <c r="E56" s="6"/>
-      <c r="G56" s="7"/>
-      <c r="H56" s="7"/>
-      <c r="I56" s="7"/>
-    </row>
-    <row r="57" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="24" t="s">
-        <v>61</v>
       </c>
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
@@ -2242,7 +2261,7 @@
     </row>
     <row r="58" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="24" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
@@ -2253,7 +2272,7 @@
     </row>
     <row r="59" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
@@ -2263,17 +2282,17 @@
       <c r="I59" s="7"/>
     </row>
     <row r="60" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="12"/>
-      <c r="B60" s="9"/>
-      <c r="C60" s="13"/>
-      <c r="D60" s="13"/>
-      <c r="E60" s="13"/>
-      <c r="F60" s="13"/>
-      <c r="G60" s="13"/>
-      <c r="H60" s="13"/>
-      <c r="I60" s="13"/>
-    </row>
-    <row r="61" spans="1:9" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B60" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C60" s="7"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="6"/>
+      <c r="G60" s="7"/>
+      <c r="H60" s="7"/>
+      <c r="I60" s="7"/>
+    </row>
+    <row r="61" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="12"/>
       <c r="B61" s="9"/>
       <c r="C61" s="13"/>
@@ -2295,7 +2314,7 @@
       <c r="H62" s="13"/>
       <c r="I62" s="13"/>
     </row>
-    <row r="63" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="12"/>
       <c r="B63" s="9"/>
       <c r="C63" s="13"/>
@@ -12777,6 +12796,17 @@
       <c r="G1015" s="13"/>
       <c r="H1015" s="13"/>
       <c r="I1015" s="13"/>
+    </row>
+    <row r="1016" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1016" s="12"/>
+      <c r="B1016" s="9"/>
+      <c r="C1016" s="13"/>
+      <c r="D1016" s="13"/>
+      <c r="E1016" s="13"/>
+      <c r="F1016" s="13"/>
+      <c r="G1016" s="13"/>
+      <c r="H1016" s="13"/>
+      <c r="I1016" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>